<commit_message>
Raw CDRS leaf and flower data
</commit_message>
<xml_diff>
--- a/Data/Raw/CDRS Tribulus flowers.xlsx
+++ b/Data/Raw/CDRS Tribulus flowers.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\R\Tribulus\Tribulus mericarp morphology\Tribulus-mericarp-morphology\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6E4B91-9A5E-469F-B978-2A8390917FB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B065E3C6-F599-4D55-B0FF-1FE6966F231F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="14355" windowHeight="15570" xr2:uid="{E716B34C-45E6-4F64-B48F-856D88762B29}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E716B34C-45E6-4F64-B48F-856D88762B29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AA$27</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -724,23 +721,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C2FA2F-6FDD-4315-B1AB-711377C53679}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q3" activeCellId="1" sqref="O3 Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -823,7 +816,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>40</v>
       </c>
@@ -876,7 +869,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>49</v>
       </c>
@@ -994,7 +987,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>56</v>
       </c>
@@ -1050,7 +1043,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>61</v>
       </c>
@@ -1112,7 +1105,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>62</v>
       </c>
@@ -1177,7 +1170,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>67</v>
       </c>
@@ -1236,7 +1229,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>74</v>
       </c>
@@ -1295,7 +1288,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>75</v>
       </c>
@@ -1357,7 +1350,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>76</v>
       </c>
@@ -1419,7 +1412,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>78</v>
       </c>
@@ -1481,7 +1474,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>90</v>
       </c>
@@ -1540,7 +1533,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>92</v>
       </c>
@@ -1590,7 +1583,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>96</v>
       </c>
@@ -1655,7 +1648,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>97</v>
       </c>
@@ -1717,7 +1710,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>102</v>
       </c>
@@ -1776,7 +1769,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>103</v>
       </c>
@@ -1835,7 +1828,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>108</v>
       </c>
@@ -1894,7 +1887,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>115</v>
       </c>
@@ -1956,7 +1949,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>117</v>
       </c>
@@ -2018,7 +2011,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>119</v>
       </c>
@@ -2077,7 +2070,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>120</v>
       </c>
@@ -2136,7 +2129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>128</v>
       </c>
@@ -2195,7 +2188,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>131</v>
       </c>
@@ -2260,7 +2253,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>141</v>
       </c>
@@ -2319,7 +2312,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>148</v>
       </c>
@@ -2382,13 +2375,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA27" xr:uid="{3846ED35-A4C2-4E9F-AB7E-55EE9AF58D6A}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="3183"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>